<commit_message>
changement regression supra eq1
</commit_message>
<xml_diff>
--- a/data/tempeallen.xlsx
+++ b/data/tempeallen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Documents\GitHub\phys_exp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD7FAF1-3F95-438A-A313-1FE379EE79A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E96F3C-AC1A-4E20-8ACA-7FF6C46D0509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9317C390-3D87-4FE5-8449-C6828F30E0E4}"/>
   </bookViews>
@@ -431,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827CC73B-E7CA-4FC1-B79B-C6102205C8CC}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,7 +504,7 @@
         <v>168</v>
       </c>
       <c r="J2">
-        <f>H2+273.15</f>
+        <f t="shared" ref="J2:J34" si="0">H2+273.15</f>
         <v>265.25</v>
       </c>
       <c r="M2">
@@ -548,7 +548,7 @@
         <v>167.4</v>
       </c>
       <c r="J3">
-        <f>H3+273.15</f>
+        <f t="shared" si="0"/>
         <v>266.25</v>
       </c>
       <c r="M3">
@@ -556,34 +556,34 @@
         <v>10</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N40" si="0">22.4 + (-196 - 22.4 )*EXP(-M3/139)</f>
+        <f t="shared" ref="N3:N40" si="1">22.4 + (-196 - 22.4 )*EXP(-M3/139)</f>
         <v>-180.83964455429214</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A51" si="1">A3+3</f>
+        <f t="shared" ref="A4:A51" si="2">A3+3</f>
         <v>6</v>
       </c>
       <c r="B4">
         <v>-5.5</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C7" si="2">C3+10</f>
+        <f t="shared" ref="C4:C7" si="3">C3+10</f>
         <v>20</v>
       </c>
       <c r="D4">
         <v>3.4</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E39" si="3">E3+10</f>
+        <f t="shared" ref="E4:E39" si="4">E3+10</f>
         <v>20</v>
       </c>
       <c r="F4">
         <v>4.4000000000000004</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G34" si="4">G3+10</f>
+        <f t="shared" ref="G4:G34" si="5">G3+10</f>
         <v>20.00001</v>
       </c>
       <c r="H4">
@@ -593,42 +593,42 @@
         <v>165.05</v>
       </c>
       <c r="J4">
-        <f>H4+273.15</f>
+        <f t="shared" si="0"/>
         <v>266.64999999999998</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M52" si="5">M3+10</f>
+        <f t="shared" ref="M4:M52" si="6">M3+10</f>
         <v>20</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-166.73165347323723</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="B5">
         <v>-5.4</v>
       </c>
       <c r="C5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F5">
         <v>5.9</v>
       </c>
       <c r="G5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30.00001</v>
       </c>
       <c r="H5">
@@ -638,42 +638,42 @@
         <v>164.78</v>
       </c>
       <c r="J5">
-        <f>H5+273.15</f>
+        <f t="shared" si="0"/>
         <v>269.95</v>
       </c>
       <c r="M5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-153.60297630891159</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="B6">
         <v>-5</v>
       </c>
       <c r="C6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="D6">
         <v>5.5</v>
       </c>
       <c r="E6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="F6">
         <v>7.2</v>
       </c>
       <c r="G6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>40.000010000000003</v>
       </c>
       <c r="H6">
@@ -683,42 +683,42 @@
         <v>164.54</v>
       </c>
       <c r="J6">
-        <f>H6+273.15</f>
+        <f t="shared" si="0"/>
         <v>272.75</v>
       </c>
       <c r="M6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-141.38563345018633</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="B7">
         <v>-4.5</v>
       </c>
       <c r="C7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="D7">
         <v>5.6</v>
       </c>
       <c r="E7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="F7">
         <v>8.3000000000000007</v>
       </c>
       <c r="G7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>50.000010000000003</v>
       </c>
       <c r="H7">
@@ -728,21 +728,21 @@
         <v>164.36</v>
       </c>
       <c r="J7">
-        <f>H7+273.15</f>
+        <f t="shared" si="0"/>
         <v>274.95</v>
       </c>
       <c r="M7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-130.01636412781798</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="B8">
@@ -756,14 +756,14 @@
         <v>6.4</v>
       </c>
       <c r="E8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="F8">
         <v>9.4</v>
       </c>
       <c r="G8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>60.000010000000003</v>
       </c>
       <c r="H8">
@@ -773,42 +773,42 @@
         <v>164.29</v>
       </c>
       <c r="J8">
-        <f>H8+273.15</f>
+        <f t="shared" si="0"/>
         <v>276.54999999999995</v>
       </c>
       <c r="M8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="N8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-119.43629885345828</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="B9">
         <v>-4.0999999999999996</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C23" si="6">C8+10</f>
+        <f t="shared" ref="C9:C23" si="7">C8+10</f>
         <v>80</v>
       </c>
       <c r="D9">
         <v>6.8</v>
       </c>
       <c r="E9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="F9">
         <v>9.3000000000000007</v>
       </c>
       <c r="G9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>70.000010000000003</v>
       </c>
       <c r="H9">
@@ -818,42 +818,42 @@
         <v>164.22</v>
       </c>
       <c r="J9">
-        <f>H9+273.15</f>
+        <f t="shared" si="0"/>
         <v>278.95</v>
       </c>
       <c r="M9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="N9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-109.59065459648909</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B10">
         <v>-3.9</v>
       </c>
       <c r="C10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
       <c r="D10">
         <v>6.4</v>
       </c>
       <c r="E10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="F10">
         <v>9.1999999999999993</v>
       </c>
       <c r="G10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>80.000010000000003</v>
       </c>
       <c r="H10">
@@ -863,42 +863,42 @@
         <v>164.17</v>
       </c>
       <c r="J10">
-        <f>H10+273.15</f>
+        <f t="shared" si="0"/>
         <v>279.04999999999995</v>
       </c>
       <c r="M10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="N10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-100.42845112032415</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="B11">
         <v>-3.6</v>
       </c>
       <c r="C11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="D11">
         <v>6.3</v>
       </c>
       <c r="E11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="F11">
         <v>10.3</v>
       </c>
       <c r="G11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90.000010000000003</v>
       </c>
       <c r="H11">
@@ -908,42 +908,42 @@
         <v>164.17</v>
       </c>
       <c r="J11">
-        <f>H11+273.15</f>
+        <f t="shared" si="0"/>
         <v>278.14999999999998</v>
       </c>
       <c r="M11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="N11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-91.90224700938154</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B12">
         <v>-3.4</v>
       </c>
       <c r="C12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>110</v>
       </c>
       <c r="D12">
         <v>6.4</v>
       </c>
       <c r="E12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="F12">
         <v>10.9</v>
       </c>
       <c r="G12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100.00001</v>
       </c>
       <c r="H12">
@@ -953,42 +953,42 @@
         <v>164.14</v>
       </c>
       <c r="J12">
-        <f>H12+273.15</f>
+        <f t="shared" si="0"/>
         <v>279.54999999999995</v>
       </c>
       <c r="M12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="N12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-83.967894019888291</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B13">
         <v>-3</v>
       </c>
       <c r="C13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
       <c r="D13">
         <v>6.6</v>
       </c>
       <c r="E13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
       <c r="F13">
         <v>9.3000000000000007</v>
       </c>
       <c r="G13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>110.00001</v>
       </c>
       <c r="H13">
@@ -998,42 +998,42 @@
         <v>164.12</v>
       </c>
       <c r="J13">
-        <f>H13+273.15</f>
+        <f t="shared" si="0"/>
         <v>280.84999999999997</v>
       </c>
       <c r="M13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="N13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-76.584308482558214</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="B14">
         <v>-2.9</v>
       </c>
       <c r="C14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>130</v>
       </c>
       <c r="D14">
         <v>6</v>
       </c>
       <c r="E14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="F14">
         <v>10</v>
       </c>
       <c r="G14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>120.00001</v>
       </c>
       <c r="H14">
@@ -1043,42 +1043,42 @@
         <v>164.12</v>
       </c>
       <c r="J14">
-        <f>H14+273.15</f>
+        <f t="shared" si="0"/>
         <v>281.84999999999997</v>
       </c>
       <c r="M14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>120</v>
       </c>
       <c r="N14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-69.713258573477731</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="B15">
         <v>-2.5</v>
       </c>
       <c r="C15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
       <c r="D15">
         <v>6.7</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130</v>
       </c>
       <c r="F15">
         <v>10.5</v>
       </c>
       <c r="G15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>130.00001</v>
       </c>
       <c r="H15">
@@ -1088,15 +1088,15 @@
         <v>164.11</v>
       </c>
       <c r="J15">
-        <f>H15+273.15</f>
+        <f t="shared" si="0"/>
         <v>282.14999999999998</v>
       </c>
       <c r="M15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>130</v>
       </c>
       <c r="N15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-63.319166351699714</v>
       </c>
     </row>
@@ -1108,21 +1108,21 @@
         <v>-1.6</v>
       </c>
       <c r="C16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="D16">
         <v>7.2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
       <c r="F16">
         <v>10.5</v>
       </c>
       <c r="G16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>140.00001</v>
       </c>
       <c r="H16">
@@ -1132,42 +1132,42 @@
         <v>164.07</v>
       </c>
       <c r="J16">
-        <f>H16+273.15</f>
+        <f t="shared" si="0"/>
         <v>283.95</v>
       </c>
       <c r="M16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="N16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-57.368923538505904</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="B17">
         <v>-1.5</v>
       </c>
       <c r="C17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>160</v>
       </c>
       <c r="D17">
         <v>7.8</v>
       </c>
       <c r="E17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="F17">
         <v>11.4</v>
       </c>
       <c r="G17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150.00001</v>
       </c>
       <c r="H17">
@@ -1177,15 +1177,15 @@
         <v>164.07</v>
       </c>
       <c r="J17">
-        <f>H17+273.15</f>
+        <f t="shared" si="0"/>
         <v>284.54999999999995</v>
       </c>
       <c r="M17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="N17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-51.831720084452606</v>
       </c>
     </row>
@@ -1198,21 +1198,21 @@
         <v>-1.2</v>
       </c>
       <c r="C18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>170</v>
       </c>
       <c r="D18">
         <v>7.7</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>160</v>
       </c>
       <c r="F18">
         <v>12</v>
       </c>
       <c r="G18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>160.00001</v>
       </c>
       <c r="H18">
@@ -1222,42 +1222,42 @@
         <v>164.08</v>
       </c>
       <c r="J18">
-        <f>H18+273.15</f>
+        <f t="shared" si="0"/>
         <v>283.95</v>
       </c>
       <c r="M18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>160</v>
       </c>
       <c r="N18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-46.678884636528643</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="B19">
         <v>-0.7</v>
       </c>
       <c r="C19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>180</v>
       </c>
       <c r="D19">
         <v>7.9</v>
       </c>
       <c r="E19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>170</v>
       </c>
       <c r="F19">
         <v>12.4</v>
       </c>
       <c r="G19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>170.00001</v>
       </c>
       <c r="H19">
@@ -1267,42 +1267,42 @@
         <v>164.08</v>
       </c>
       <c r="J19">
-        <f>H19+273.15</f>
+        <f t="shared" si="0"/>
         <v>283.45</v>
       </c>
       <c r="M19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>170</v>
       </c>
       <c r="N19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-41.883736079372873</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="B20">
         <v>-0.1</v>
       </c>
       <c r="C20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>190</v>
       </c>
       <c r="D20">
         <v>7.9</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
       <c r="F20">
         <v>13.1</v>
       </c>
       <c r="G20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>180.00001</v>
       </c>
       <c r="H20">
@@ -1312,42 +1312,42 @@
         <v>164.09</v>
       </c>
       <c r="J20">
-        <f>H20+273.15</f>
+        <f t="shared" si="0"/>
         <v>284.25</v>
       </c>
       <c r="M20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>180</v>
       </c>
       <c r="N20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-37.421445381839135</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="B21">
         <v>-0.2</v>
       </c>
       <c r="C21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>200</v>
       </c>
       <c r="D21">
         <v>7.6</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>190</v>
       </c>
       <c r="F21">
         <v>13.2</v>
       </c>
       <c r="G21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>190.00001</v>
       </c>
       <c r="H21">
@@ -1357,42 +1357,42 @@
         <v>164.1</v>
       </c>
       <c r="J21">
-        <f>H21+273.15</f>
+        <f t="shared" si="0"/>
         <v>285.04999999999995</v>
       </c>
       <c r="M21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>190</v>
       </c>
       <c r="N21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-33.268907033557639</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="B22">
         <v>-0.3</v>
       </c>
       <c r="C22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>210</v>
       </c>
       <c r="D22">
         <v>7.9</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="F22">
         <v>13.3</v>
       </c>
       <c r="G22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>200.00001</v>
       </c>
       <c r="H22">
@@ -1402,15 +1402,15 @@
         <v>164.11</v>
       </c>
       <c r="J22">
-        <f>H22+273.15</f>
+        <f t="shared" si="0"/>
         <v>285.34999999999997</v>
       </c>
       <c r="M22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="N22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-29.404619405797561</v>
       </c>
     </row>
@@ -1423,21 +1423,21 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>220</v>
       </c>
       <c r="D23">
         <v>8</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>210</v>
       </c>
       <c r="F23">
         <v>13.7</v>
       </c>
       <c r="G23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>210.00001</v>
       </c>
       <c r="H23">
@@ -1447,21 +1447,21 @@
         <v>164.1</v>
       </c>
       <c r="J23">
-        <f>H23+273.15</f>
+        <f t="shared" si="0"/>
         <v>285.75</v>
       </c>
       <c r="M23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>210</v>
       </c>
       <c r="N23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-25.808573417145986</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="B24">
@@ -1475,14 +1475,14 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="E24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>220</v>
       </c>
       <c r="F24">
         <v>13.9</v>
       </c>
       <c r="G24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>220.00001</v>
       </c>
       <c r="H24">
@@ -1492,42 +1492,42 @@
         <v>164.1</v>
       </c>
       <c r="J24">
-        <f>H24+273.15</f>
+        <f t="shared" si="0"/>
         <v>286.14999999999998</v>
       </c>
       <c r="M24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>220</v>
       </c>
       <c r="N24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-22.462148927519443</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="B25">
         <v>1.2</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:C30" si="7">C24+10</f>
+        <f t="shared" ref="C25:C30" si="8">C24+10</f>
         <v>250</v>
       </c>
       <c r="D25">
         <v>9.3000000000000007</v>
       </c>
       <c r="E25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>230</v>
       </c>
       <c r="F25">
         <v>13.7</v>
       </c>
       <c r="G25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>230.00001</v>
       </c>
       <c r="H25">
@@ -1537,15 +1537,15 @@
         <v>164.11</v>
       </c>
       <c r="J25">
-        <f>H25+273.15</f>
+        <f t="shared" si="0"/>
         <v>287.34999999999997</v>
       </c>
       <c r="M25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>230</v>
       </c>
       <c r="N25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-19.348018324041988</v>
       </c>
     </row>
@@ -1557,21 +1557,21 @@
         <v>1.5</v>
       </c>
       <c r="C26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>260</v>
       </c>
       <c r="D26">
         <v>9.8000000000000007</v>
       </c>
       <c r="E26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="F26">
         <v>13.5</v>
       </c>
       <c r="G26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>240.00001</v>
       </c>
       <c r="H26">
@@ -1581,35 +1581,35 @@
         <v>164.09</v>
       </c>
       <c r="J26">
-        <f>H26+273.15</f>
+        <f t="shared" si="0"/>
         <v>287.95</v>
       </c>
       <c r="M26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>240</v>
       </c>
       <c r="N26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-16.450056799562127</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="B27">
         <v>1.6</v>
       </c>
       <c r="C27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>270</v>
       </c>
       <c r="D27">
         <v>10</v>
       </c>
       <c r="E27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>250</v>
       </c>
       <c r="F27">
@@ -1626,42 +1626,42 @@
         <v>164.1</v>
       </c>
       <c r="J27">
-        <f>H27+273.15</f>
+        <f t="shared" si="0"/>
         <v>288.64999999999998</v>
       </c>
       <c r="M27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>250</v>
       </c>
       <c r="N27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-13.753258859235657</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="B28">
         <v>1.9</v>
       </c>
       <c r="C28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>280</v>
       </c>
       <c r="D28">
         <v>10.199999999999999</v>
       </c>
       <c r="E28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>260</v>
       </c>
       <c r="F28">
         <v>14.3</v>
       </c>
       <c r="G28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>260.00000999999997</v>
       </c>
       <c r="H28">
@@ -1671,42 +1671,42 @@
         <v>164.1</v>
       </c>
       <c r="J28">
-        <f>H28+273.15</f>
+        <f t="shared" si="0"/>
         <v>288.95</v>
       </c>
       <c r="M28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>260</v>
       </c>
       <c r="N28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-11.243660622849674</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="B29">
         <v>1.9</v>
       </c>
       <c r="C29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>290</v>
       </c>
       <c r="D29">
         <v>10.3</v>
       </c>
       <c r="E29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>270</v>
       </c>
       <c r="F29">
         <v>14.6</v>
       </c>
       <c r="G29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>270.00000999999997</v>
       </c>
       <c r="H29">
@@ -1716,7 +1716,7 @@
         <v>164.09</v>
       </c>
       <c r="J29">
-        <f>H29+273.15</f>
+        <f t="shared" si="0"/>
         <v>289.54999999999995</v>
       </c>
       <c r="M29">
@@ -1737,21 +1737,21 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>300</v>
       </c>
       <c r="D30">
         <v>10.7</v>
       </c>
       <c r="E30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>280</v>
       </c>
       <c r="F30">
         <v>14.7</v>
       </c>
       <c r="G30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>280.00000999999997</v>
       </c>
       <c r="H30">
@@ -1761,21 +1761,21 @@
         <v>164.09</v>
       </c>
       <c r="J30">
-        <f>H30+273.15</f>
+        <f t="shared" si="0"/>
         <v>289.95</v>
       </c>
       <c r="M30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>280</v>
       </c>
       <c r="N30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6.7349870077472609</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="B31">
@@ -1789,14 +1789,14 @@
         <v>11</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>290</v>
       </c>
       <c r="F31">
         <v>15</v>
       </c>
       <c r="G31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>290.00000999999997</v>
       </c>
       <c r="H31">
@@ -1806,7 +1806,7 @@
         <v>164.09</v>
       </c>
       <c r="J31">
-        <f>H31+273.15</f>
+        <f t="shared" si="0"/>
         <v>290.34999999999997</v>
       </c>
       <c r="M31">
@@ -1814,34 +1814,34 @@
         <v>290</v>
       </c>
       <c r="N31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4.7125659503135218</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="B32">
         <v>2.2000000000000002</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:C50" si="8">C31+10</f>
+        <f t="shared" ref="C32:C50" si="9">C31+10</f>
         <v>370</v>
       </c>
       <c r="D32">
         <v>10.8</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="F32">
         <v>14.7</v>
       </c>
       <c r="G32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>300.00000999999997</v>
       </c>
       <c r="H32">
@@ -1851,42 +1851,42 @@
         <v>164.1</v>
       </c>
       <c r="J32">
-        <f>H32+273.15</f>
+        <f t="shared" si="0"/>
         <v>290.14999999999998</v>
       </c>
       <c r="M32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="N32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.8305323566690639</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="B33">
         <v>2.6</v>
       </c>
       <c r="C33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>380</v>
       </c>
       <c r="D33">
         <v>11</v>
       </c>
       <c r="E33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>310</v>
       </c>
       <c r="F33">
         <v>15</v>
       </c>
       <c r="G33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>310.00000999999997</v>
       </c>
       <c r="H33">
@@ -1896,42 +1896,42 @@
         <v>164.1</v>
       </c>
       <c r="J33">
-        <f>H33+273.15</f>
+        <f t="shared" si="0"/>
         <v>290.54999999999995</v>
       </c>
       <c r="M33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>310</v>
       </c>
       <c r="N33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.0791411542352911</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>108</v>
       </c>
       <c r="B34">
         <v>2.9</v>
       </c>
       <c r="C34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>390</v>
       </c>
       <c r="D34">
         <v>11.1</v>
       </c>
       <c r="E34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>320</v>
       </c>
       <c r="F34">
         <v>15.4</v>
       </c>
       <c r="G34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>320.00000999999997</v>
       </c>
       <c r="H34">
@@ -1941,214 +1941,220 @@
         <v>164.8</v>
       </c>
       <c r="J34">
-        <f>H34+273.15</f>
+        <f t="shared" si="0"/>
         <v>291.04999999999995</v>
       </c>
       <c r="M34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>320</v>
       </c>
       <c r="N34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.55067627002365782</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111</v>
       </c>
       <c r="B35">
         <v>3.2</v>
       </c>
       <c r="C35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>400</v>
       </c>
       <c r="D35">
         <v>11.2</v>
       </c>
       <c r="E35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>330</v>
       </c>
       <c r="F35">
         <v>15.7</v>
       </c>
+      <c r="I35">
+        <v>207</v>
+      </c>
+      <c r="J35">
+        <v>77.36</v>
+      </c>
       <c r="M35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>330</v>
       </c>
       <c r="N35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0673590264100135</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>114</v>
       </c>
       <c r="B36">
         <v>3.2</v>
       </c>
       <c r="C36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>410</v>
       </c>
       <c r="D36">
         <v>11.1</v>
       </c>
       <c r="E36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>340</v>
       </c>
       <c r="F36">
         <v>15.8</v>
       </c>
       <c r="M36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>340</v>
       </c>
       <c r="N36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.4787604197689319</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>117</v>
       </c>
       <c r="B37">
         <v>3.2</v>
       </c>
       <c r="C37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>420</v>
       </c>
       <c r="D37">
         <v>11.4</v>
       </c>
       <c r="E37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>350</v>
       </c>
       <c r="F37">
         <v>15.6</v>
       </c>
       <c r="M37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>350</v>
       </c>
       <c r="N37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.7921886134946625</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="B38">
         <v>3.4</v>
       </c>
       <c r="C38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>430</v>
       </c>
       <c r="D38">
         <v>11.4</v>
       </c>
       <c r="E38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>360</v>
       </c>
       <c r="F38">
         <v>15.8</v>
       </c>
       <c r="M38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>360</v>
       </c>
       <c r="N38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.0144444708225144</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123</v>
       </c>
       <c r="B39">
         <v>3.6</v>
       </c>
       <c r="C39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>440</v>
       </c>
       <c r="D39">
         <v>11.5</v>
       </c>
       <c r="E39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>370</v>
       </c>
       <c r="F39">
         <v>16</v>
       </c>
       <c r="M39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>370</v>
       </c>
       <c r="N39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1518567693468462</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="B40">
         <v>3.9</v>
       </c>
       <c r="C40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>450</v>
       </c>
       <c r="D40">
         <v>11.8</v>
       </c>
       <c r="M40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>380</v>
       </c>
       <c r="N40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.2103149711040153</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>129</v>
       </c>
       <c r="B41">
         <v>3.7</v>
       </c>
       <c r="C41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>460</v>
       </c>
       <c r="D41">
         <v>12.8</v>
       </c>
       <c r="M41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>390</v>
       </c>
       <c r="N41">
@@ -2158,244 +2164,244 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>132</v>
       </c>
       <c r="B42">
         <v>3.8</v>
       </c>
       <c r="C42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>470</v>
       </c>
       <c r="D42">
         <v>12.6</v>
       </c>
       <c r="M42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>400</v>
       </c>
       <c r="N42">
-        <f t="shared" ref="N42:N52" si="9">22.4 + (-196 - 22.4 )*EXP(-M42/139)</f>
+        <f t="shared" ref="N42:N52" si="10">22.4 + (-196 - 22.4 )*EXP(-M42/139)</f>
         <v>10.111911209800653</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>135</v>
       </c>
       <c r="B43">
         <v>3.6</v>
       </c>
       <c r="C43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>480</v>
       </c>
       <c r="D43">
         <v>12.2</v>
       </c>
       <c r="M43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>410</v>
       </c>
       <c r="N43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10.964895613682705</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>138</v>
       </c>
       <c r="B44">
         <v>3.8</v>
       </c>
       <c r="C44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>490</v>
       </c>
       <c r="D44">
         <v>11.2</v>
       </c>
       <c r="M44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>420</v>
       </c>
       <c r="N44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11.758669638661383</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>141</v>
       </c>
       <c r="B45">
         <v>4.0999999999999996</v>
       </c>
       <c r="C45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>500</v>
       </c>
       <c r="D45">
         <v>12.4</v>
       </c>
       <c r="M45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>430</v>
       </c>
       <c r="N45">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.497343405571163</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="B46">
         <v>4.5999999999999996</v>
       </c>
       <c r="C46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>510</v>
       </c>
       <c r="D46">
         <v>12.3</v>
       </c>
       <c r="M46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>440</v>
       </c>
       <c r="N46">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13.184741728960926</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>147</v>
       </c>
       <c r="B47">
         <v>4.8</v>
       </c>
       <c r="C47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>520</v>
       </c>
       <c r="D47">
         <v>12.5</v>
       </c>
       <c r="M47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>450</v>
       </c>
       <c r="N47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13.824423921785796</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="B48">
         <v>4.5999999999999996</v>
       </c>
       <c r="C48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>530</v>
       </c>
       <c r="D48">
         <v>12.8</v>
       </c>
       <c r="M48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>460</v>
       </c>
       <c r="N48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14.419702225345487</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>153</v>
       </c>
       <c r="B49">
         <v>4.5</v>
       </c>
       <c r="C49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>540</v>
       </c>
       <c r="D49">
         <v>13.1</v>
       </c>
       <c r="M49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>470</v>
       </c>
       <c r="N49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14.973658959898389</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>156</v>
       </c>
       <c r="B50">
         <v>4.5999999999999996</v>
       </c>
       <c r="C50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>550</v>
       </c>
       <c r="D50">
         <v>13.7</v>
       </c>
       <c r="M50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>480</v>
       </c>
       <c r="N50">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.489162484756392</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>159</v>
       </c>
       <c r="B51">
         <v>4.5</v>
       </c>
       <c r="M51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>490</v>
       </c>
       <c r="N51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.968882050501016</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>500</v>
       </c>
       <c r="N52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>16.41530162022481</v>
       </c>
     </row>

</xml_diff>